<commit_message>
TPU branch codes are updated according to the latest main repo updates.
</commit_message>
<xml_diff>
--- a/inference_zeroshot/aurocs.xlsx
+++ b/inference_zeroshot/aurocs.xlsx
@@ -489,58 +489,58 @@
     </row>
     <row r="2" spans="1:18">
       <c r="A2">
-        <v>0.5425359477124183</v>
+        <v>0.5419433551198256</v>
       </c>
       <c r="B2">
-        <v>0.6641583054626533</v>
+        <v>0.6641670150501673</v>
       </c>
       <c r="C2">
-        <v>0.6636681659170415</v>
+        <v>0.663893859521852</v>
       </c>
       <c r="D2">
-        <v>0.4811766623207301</v>
+        <v>0.4828335506301608</v>
       </c>
       <c r="E2">
-        <v>0.6360929902660731</v>
+        <v>0.6374928838741589</v>
       </c>
       <c r="F2">
-        <v>0.5840680443470012</v>
+        <v>0.5828862869493555</v>
       </c>
       <c r="G2">
-        <v>0.5516821836648328</v>
+        <v>0.5532074340527579</v>
       </c>
       <c r="H2">
-        <v>0.60240625</v>
+        <v>0.6011145833333333</v>
       </c>
       <c r="I2">
-        <v>0.5686811031344395</v>
+        <v>0.5694558863912753</v>
       </c>
       <c r="J2">
-        <v>0.5083988126418718</v>
+        <v>0.5084826261568011</v>
       </c>
       <c r="K2">
-        <v>0.5398343721144967</v>
+        <v>0.5391490650969528</v>
       </c>
       <c r="L2">
-        <v>0.5797951913778712</v>
+        <v>0.5798613119984131</v>
       </c>
       <c r="M2">
-        <v>0.5681453850422344</v>
+        <v>0.5675596522596955</v>
       </c>
       <c r="N2">
-        <v>0.6113277468956553</v>
+        <v>0.6113000912635859</v>
       </c>
       <c r="O2">
-        <v>0.5182772651919825</v>
+        <v>0.5189638138615851</v>
       </c>
       <c r="P2">
-        <v>0.5053886772853187</v>
+        <v>0.5059188885041551</v>
       </c>
       <c r="Q2">
-        <v>0.5336122004357299</v>
+        <v>0.5342396514161221</v>
       </c>
       <c r="R2">
-        <v>0.6417858301514812</v>
+        <v>0.6426093683711411</v>
       </c>
     </row>
   </sheetData>

</xml_diff>